<commit_message>
change in the bar chart
</commit_message>
<xml_diff>
--- a/GlobalSales/ram_data.xlsx
+++ b/GlobalSales/ram_data.xlsx
@@ -589,12 +589,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx2"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -622,12 +619,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx2"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -660,9 +654,32 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -863,8 +880,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
         <c:axId val="479282360"/>
         <c:axId val="479577168"/>
       </c:barChart>
@@ -883,7 +900,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
+              <a:schemeClr val="tx2">
                 <a:lumMod val="15000"/>
                 <a:lumOff val="85000"/>
               </a:schemeClr>
@@ -899,10 +916,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx2"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -930,7 +944,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="tx2">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -958,10 +972,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx2"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -993,7 +1004,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="tx2">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -1061,33 +1072,27 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1102,7 +1107,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1110,7 +1115,7 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1118,17 +1123,14 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
@@ -1137,9 +1139,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
@@ -1162,35 +1163,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="31750" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1199,33 +1200,32 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="12700">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="lt2"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1241,21 +1241,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1289,17 +1284,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -1308,14 +1303,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1327,26 +1322,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1360,96 +1349,99 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1457,17 +1449,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:seriesLine>
@@ -1476,12 +1468,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1490,14 +1479,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1506,10 +1495,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
@@ -1518,7 +1504,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1539,10 +1525,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
@@ -1551,14 +1534,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1567,16 +1544,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1864,7 +1841,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>